<commit_message>
updated location of images src seed data
</commit_message>
<xml_diff>
--- a/app/assets/data/Courses.xlsx
+++ b/app/assets/data/Courses.xlsx
@@ -27,34 +27,34 @@
     <t>A guided tour of the entire universe. Over the course of this series we’ll explore planets, stars, black holes, galaxies, subatomic particles, and even the eventual fate of the Universe itself.</t>
   </si>
   <si>
-    <t>assets/Course1.png</t>
-  </si>
-  <si>
     <t>World History</t>
   </si>
   <si>
     <t>In a mere fifteen thousand years, humans went from hunting and gathering to creating such improbabilities as the airplane, the Internet, and the ninety-nine cent double cheeseburger. Learn about that journey in this course.</t>
   </si>
   <si>
-    <t>assets/Course2.png</t>
-  </si>
-  <si>
     <t>Chemistry</t>
   </si>
   <si>
     <t>Chemistry holds the secrets to how life first formed, how cancers are cured, how iPhones have bigger hard drives than 5 year old laptops and how life on this planet might just be able to continue thriving, even ours, if we play our cards right. Chemistry is the science of how three tiny particles, the proton, the neutron and the electron came together in trillions of combinations to form, everything.</t>
   </si>
   <si>
-    <t>assets/Course3.png</t>
-  </si>
-  <si>
     <t>Biology</t>
   </si>
   <si>
     <t>Come today to learn about covalent and ionic and hydrogen bonds. What about electron orbitals and the octet rule and what does it all have to do with a mad man named Gilbert Lewis? It’s all contained within.</t>
   </si>
   <si>
-    <t>assets/Course4.png</t>
+    <t>Course1.png</t>
+  </si>
+  <si>
+    <t>Course2.png</t>
+  </si>
+  <si>
+    <t>Course3.png</t>
+  </si>
+  <si>
+    <t>Course4.png</t>
   </si>
 </sst>
 </file>
@@ -374,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -388,37 +388,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="375">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="409">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="360">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
added chapter link to section view
</commit_message>
<xml_diff>
--- a/app/assets/data/Courses.xlsx
+++ b/app/assets/data/Courses.xlsx
@@ -364,7 +364,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -374,13 +374,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="315">
+    <row r="1" spans="1:3" ht="90">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,7 +396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="375">
+    <row r="2" spans="1:3" ht="105">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -402,7 +407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="409">
+    <row r="3" spans="1:3" ht="195">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -413,7 +418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="360">
+    <row r="4" spans="1:3" ht="105">
       <c r="A4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Edit mode for courses fully working. Still need to fix html issues on chapter edit mode.
</commit_message>
<xml_diff>
--- a/app/assets/data/Courses.xlsx
+++ b/app/assets/data/Courses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -364,7 +367,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -385,7 +388,7 @@
     <col min="3" max="3" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="90">
+    <row r="1" spans="1:6" ht="90">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,8 +398,11 @@
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="105">
+    <row r="2" spans="1:6" ht="105">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -406,8 +412,12 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="195">
+    <row r="3" spans="1:6" ht="195">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -417,8 +427,11 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="105">
+    <row r="4" spans="1:6" ht="105">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -427,6 +440,9 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attempt to fix duplicate bug
</commit_message>
<xml_diff>
--- a/app/assets/data/Courses.xlsx
+++ b/app/assets/data/Courses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -378,7 +378,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -399,7 +399,7 @@
         <v>8</v>
       </c>
       <c r="D1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="105">
@@ -413,7 +413,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2"/>
     </row>

</xml_diff>